<commit_message>
Add filtering & extract charts to separate page
</commit_message>
<xml_diff>
--- a/Liftee/Liftee/wwwroot/files/Пример даш борд.xlsx
+++ b/Liftee/Liftee/wwwroot/files/Пример даш борд.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miraziz_Khidoyatov\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73663F12-F829-4DF2-8CFF-F7990177D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F127D6E3-3545-448B-AB81-C8D23616758A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7CE04CA5-089B-4D7D-A037-97AC07C0C0E2}"/>
   </bookViews>
@@ -1068,7 +1068,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E8CD51F-6419-477F-9BD2-1556561E12D3}">
   <dimension ref="A1:W160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1079,7 +1081,7 @@
     <col min="5" max="5" width="16.6640625" customWidth="1"/>
     <col min="6" max="6" width="17.88671875" customWidth="1"/>
     <col min="7" max="7" width="19.5546875" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" customWidth="1"/>
     <col min="9" max="9" width="17.33203125" customWidth="1"/>
     <col min="10" max="10" width="21.6640625" customWidth="1"/>
     <col min="11" max="11" width="13.109375" customWidth="1"/>
@@ -6206,7 +6208,7 @@
       <c r="P124" s="4"/>
       <c r="Q124" s="4"/>
     </row>
-    <row r="125" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="6">
         <v>124</v>
       </c>
@@ -6235,7 +6237,7 @@
       <c r="P125" s="7"/>
       <c r="Q125" s="7"/>
     </row>
-    <row r="126" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="3">
         <v>125</v>
       </c>
@@ -6262,7 +6264,7 @@
       <c r="P126" s="4"/>
       <c r="Q126" s="4"/>
     </row>
-    <row r="127" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="6">
         <v>126</v>
       </c>
@@ -6289,7 +6291,7 @@
       <c r="P127" s="7"/>
       <c r="Q127" s="7"/>
     </row>
-    <row r="128" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="3">
         <v>127</v>
       </c>
@@ -6316,7 +6318,7 @@
       <c r="P128" s="4"/>
       <c r="Q128" s="4"/>
     </row>
-    <row r="129" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="6">
         <v>128</v>
       </c>
@@ -6640,7 +6642,7 @@
       <c r="P138" s="4"/>
       <c r="Q138" s="4"/>
     </row>
-    <row r="139" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A139" s="6">
         <v>138</v>
       </c>
@@ -6667,7 +6669,7 @@
       <c r="P139" s="7"/>
       <c r="Q139" s="7"/>
     </row>
-    <row r="140" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="3">
         <v>139</v>
       </c>
@@ -6700,7 +6702,7 @@
       <c r="P140" s="4"/>
       <c r="Q140" s="4"/>
     </row>
-    <row r="141" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="6">
         <v>140</v>
       </c>
@@ -6733,7 +6735,7 @@
       <c r="P141" s="7"/>
       <c r="Q141" s="7"/>
     </row>
-    <row r="142" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A142" s="3">
         <v>141</v>
       </c>
@@ -6766,7 +6768,7 @@
       <c r="P142" s="4"/>
       <c r="Q142" s="4"/>
     </row>
-    <row r="143" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A143" s="6">
         <v>142</v>
       </c>
@@ -6799,7 +6801,7 @@
       <c r="P143" s="7"/>
       <c r="Q143" s="7"/>
     </row>
-    <row r="144" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A144" s="3">
         <v>143</v>
       </c>
@@ -6832,7 +6834,7 @@
       <c r="P144" s="4"/>
       <c r="Q144" s="4"/>
     </row>
-    <row r="145" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A145" s="6">
         <v>144</v>
       </c>
@@ -6865,7 +6867,7 @@
       <c r="P145" s="7"/>
       <c r="Q145" s="7"/>
     </row>
-    <row r="146" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="3">
         <v>145</v>
       </c>
@@ -6898,7 +6900,7 @@
       <c r="P146" s="4"/>
       <c r="Q146" s="4"/>
     </row>
-    <row r="147" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A147" s="6">
         <v>146</v>
       </c>
@@ -6931,7 +6933,7 @@
       <c r="P147" s="7"/>
       <c r="Q147" s="7"/>
     </row>
-    <row r="148" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A148" s="3">
         <v>147</v>
       </c>
@@ -6964,7 +6966,7 @@
       <c r="P148" s="4"/>
       <c r="Q148" s="4"/>
     </row>
-    <row r="149" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A149" s="6">
         <v>148</v>
       </c>
@@ -6997,7 +6999,7 @@
       <c r="P149" s="7"/>
       <c r="Q149" s="7"/>
     </row>
-    <row r="150" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A150" s="3">
         <v>149</v>
       </c>
@@ -7030,7 +7032,7 @@
       <c r="P150" s="4"/>
       <c r="Q150" s="4"/>
     </row>
-    <row r="151" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A151" s="6">
         <v>150</v>
       </c>
@@ -7063,7 +7065,7 @@
       <c r="P151" s="7"/>
       <c r="Q151" s="7"/>
     </row>
-    <row r="152" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A152" s="3">
         <v>151</v>
       </c>
@@ -7096,7 +7098,7 @@
       <c r="P152" s="4"/>
       <c r="Q152" s="4"/>
     </row>
-    <row r="153" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A153" s="6">
         <v>152</v>
       </c>
@@ -7123,7 +7125,7 @@
       <c r="P153" s="7"/>
       <c r="Q153" s="7"/>
     </row>
-    <row r="154" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A154" s="3">
         <v>153</v>
       </c>
@@ -7150,7 +7152,7 @@
       <c r="P154" s="4"/>
       <c r="Q154" s="4"/>
     </row>
-    <row r="155" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A155" s="6">
         <v>154</v>
       </c>
@@ -7183,7 +7185,7 @@
       <c r="P155" s="7"/>
       <c r="Q155" s="7"/>
     </row>
-    <row r="156" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A156" s="3">
         <v>155</v>
       </c>
@@ -7216,7 +7218,7 @@
       <c r="P156" s="4"/>
       <c r="Q156" s="4"/>
     </row>
-    <row r="157" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A157" s="6">
         <v>156</v>
       </c>
@@ -7249,7 +7251,7 @@
       <c r="P157" s="7"/>
       <c r="Q157" s="7"/>
     </row>
-    <row r="158" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A158" s="3">
         <v>157</v>
       </c>
@@ -7282,7 +7284,7 @@
       <c r="P158" s="4"/>
       <c r="Q158" s="4"/>
     </row>
-    <row r="159" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A159" s="6">
         <v>158</v>
       </c>
@@ -7309,7 +7311,7 @@
       <c r="P159" s="7"/>
       <c r="Q159" s="7"/>
     </row>
-    <row r="160" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A160" s="19">
         <v>159</v>
       </c>

</xml_diff>